<commit_message>
Type and Procedure clean-up
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestWorksheet.xlsx
+++ b/src/test/resources/Data/TestWorksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Accreditation_20230417125419</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>Contact_20230422143214</t>
+  </si>
+  <si>
+    <t>Procedure_20230422152130</t>
+  </si>
+  <si>
+    <t>Procedure_20230422152316</t>
+  </si>
+  <si>
+    <t>Procedure_20230422152845</t>
+  </si>
+  <si>
+    <t>Type_20230422153248</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1071,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A4:A9"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
@@ -1070,6 +1082,16 @@
     <col min="1" max="1" customWidth="true" width="30.7142857142857" collapsed="true"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Common method for Remember button
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestWorksheet.xlsx
+++ b/src/test/resources/Data/TestWorksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Accreditation_20230417125419</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Type_20230422153248</t>
+  </si>
+  <si>
+    <t>Type_20230422172311</t>
+  </si>
+  <si>
+    <t>Type_20230422172645</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1095,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Completed multiple Facilities creation
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestWorksheet.xlsx
+++ b/src/test/resources/Data/TestWorksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Procedure</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Accreditation</t>
   </si>
   <si>
-    <t>Accreditation_20230427135417</t>
+    <t>Accreditation_20230501105733</t>
   </si>
   <si>
     <t>Group</t>
@@ -76,34 +76,31 @@
     <t>Tool Assignment</t>
   </si>
   <si>
-    <t>Facility - Customer 1</t>
-  </si>
-  <si>
-    <t>Accreditation_20230501080329</t>
-  </si>
-  <si>
-    <t>Facility - Customer 2</t>
-  </si>
-  <si>
-    <t>Facility - Customer 3</t>
-  </si>
-  <si>
-    <t>Facility - Manufacturer</t>
-  </si>
-  <si>
-    <t>Facility - Sub Contractor</t>
-  </si>
-  <si>
-    <t>Facility - Lab 1</t>
-  </si>
-  <si>
-    <t>Facility - Lab 2</t>
-  </si>
-  <si>
-    <t>Facility - Lab 3</t>
-  </si>
-  <si>
-    <t>Jod Number</t>
+    <t>Facility_Cust1_20230501080655</t>
+  </si>
+  <si>
+    <t>Facility_Cust2_20230501104634</t>
+  </si>
+  <si>
+    <t>Facility_Cust3_20230501104637</t>
+  </si>
+  <si>
+    <t>Facility_Manufacturer_20230501104639</t>
+  </si>
+  <si>
+    <t>Facility_Subcontractor_20230501104642</t>
+  </si>
+  <si>
+    <t>Facility_Lab1_20230501104644</t>
+  </si>
+  <si>
+    <t>Facility_Lab2_20230501104647</t>
+  </si>
+  <si>
+    <t>Facility_Lab3_20230501104650</t>
+  </si>
+  <si>
+    <t>Job Number</t>
   </si>
   <si>
     <t>Manual Template</t>
@@ -113,12 +110,6 @@
   </si>
   <si>
     <t>Billing</t>
-  </si>
-  <si>
-    <t>Facility_Cust120230501080549</t>
-  </si>
-  <si>
-    <t>Facility_Cust1_20230501080655</t>
   </si>
 </sst>
 </file>
@@ -126,8 +117,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -147,6 +138,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -164,22 +179,52 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,22 +232,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,15 +246,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,45 +262,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,55 +284,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,121 +440,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,17 +510,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -552,6 +532,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -569,166 +567,159 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1056,12 +1047,13 @@
   <dimension ref="A2:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="30.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="30.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="39.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -1150,64 +1142,64 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Refresh button functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestWorksheet.xlsx
+++ b/src/test/resources/Data/TestWorksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Procedure</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Billing</t>
+  </si>
+  <si>
+    <t>Type_20230503142402</t>
+  </si>
+  <si>
+    <t>Procedure_20230503142450</t>
   </si>
 </sst>
 </file>
@@ -117,8 +123,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -1052,24 +1058,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="30.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="39.4285714285714" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.7142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.4285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
+    <row r="2">
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>